<commit_message>
Добавил Random Forest, CatBoost, XGBoost, Gradient Boosting методы и проверил через Stratified K-Fold
</commit_message>
<xml_diff>
--- a/data/processed/result.xlsx
+++ b/data/processed/result.xlsx
@@ -664,7 +664,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Запрос направлен</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -786,7 +786,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Отказ</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -1082,7 +1082,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Отказ</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -1664,7 +1664,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Отказ</t>
+          <t>Запрос направлен</t>
         </is>
       </c>
     </row>
@@ -1682,7 +1682,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Взыскание обращено</t>
+          <t>Запрос направлен</t>
         </is>
       </c>
     </row>
@@ -2821,7 +2821,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -2971,7 +2971,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Запрос направлен</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -3215,7 +3215,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -3336,7 +3336,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Взыскание обращено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -3409,7 +3409,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Обращение рассмотрено</t>
+          <t>Взыскание обращено</t>
         </is>
       </c>
     </row>
@@ -3445,7 +3445,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -3540,7 +3540,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Запрос направлен</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -3654,7 +3654,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Запрос направлен</t>
         </is>
       </c>
     </row>
@@ -4359,7 +4359,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Отказ</t>
+          <t>Запрос направлен</t>
         </is>
       </c>
     </row>
@@ -4612,7 +4612,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Взыскание обращено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -4705,7 +4705,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Обращение рассмотрено</t>
+          <t>Взыскание обращено</t>
         </is>
       </c>
     </row>
@@ -4775,7 +4775,7 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Запрос направлен</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -4826,7 +4826,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Взыскание обращено</t>
+          <t>Запрос направлен</t>
         </is>
       </c>
     </row>
@@ -4846,7 +4846,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Обращение рассмотрено</t>
+          <t>Постановление вынесено</t>
         </is>
       </c>
     </row>
@@ -4864,7 +4864,7 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Обращение рассмотрено</t>
+          <t>Взыскание обращено</t>
         </is>
       </c>
     </row>
@@ -4937,7 +4937,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Взыскание обращено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -5067,7 +5067,7 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Взыскание обращено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -6723,7 +6723,7 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Отказ</t>
+          <t>Запрос направлен</t>
         </is>
       </c>
     </row>
@@ -7703,7 +7703,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Отказ</t>
+          <t>Запрос направлен</t>
         </is>
       </c>
     </row>
@@ -8379,7 +8379,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>Обращение рассмотрено</t>
+          <t>Взыскание обращено</t>
         </is>
       </c>
     </row>
@@ -8426,7 +8426,7 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>Взыскание обращено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -8586,7 +8586,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>Отказ</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -8869,7 +8869,7 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -8908,7 +8908,7 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Взыскание обращено</t>
         </is>
       </c>
     </row>
@@ -9285,7 +9285,7 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>Обращение рассмотрено</t>
+          <t>Запрос направлен</t>
         </is>
       </c>
     </row>
@@ -9338,7 +9338,7 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>Запрос направлен</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -9451,7 +9451,7 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -9538,7 +9538,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>Запрос направлен</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -9556,7 +9556,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>Запрет действий</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -9645,7 +9645,7 @@
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -9697,7 +9697,7 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>Взыскание обращено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -9789,7 +9789,7 @@
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>Взыскание обращено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -9811,7 +9811,7 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -9847,7 +9847,7 @@
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>Взыскание обращено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -9920,7 +9920,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>Запрос направлен</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -10114,7 +10114,7 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>Обращение рассмотрено</t>
+          <t>Запрос направлен</t>
         </is>
       </c>
     </row>
@@ -10332,7 +10332,7 @@
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>Взыскание обращено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -10477,7 +10477,7 @@
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>Взыскание обращено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -10494,7 +10494,7 @@
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -11001,7 +11001,7 @@
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>Обращение рассмотрено</t>
+          <t>Запрос направлен</t>
         </is>
       </c>
     </row>
@@ -11239,7 +11239,7 @@
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>Отказ</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -11274,7 +11274,7 @@
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>Обращение рассмотрено</t>
+          <t>Взыскание обращено</t>
         </is>
       </c>
     </row>
@@ -11344,7 +11344,7 @@
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>Обращение рассмотрено</t>
+          <t>Запрос направлен</t>
         </is>
       </c>
     </row>
@@ -11361,7 +11361,7 @@
       </c>
       <c r="C279" t="inlineStr">
         <is>
-          <t>Обращение рассмотрено</t>
+          <t>Запрос направлен</t>
         </is>
       </c>
     </row>
@@ -11984,7 +11984,7 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>Взыскание обращено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -12001,7 +12001,7 @@
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -12347,7 +12347,7 @@
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>Взыскание обращено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -13509,7 +13509,7 @@
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>Запрос направлен</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -13562,7 +13562,7 @@
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>Запрос направлен</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -13920,7 +13920,7 @@
       </c>
       <c r="C364" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Взыскание обращено</t>
         </is>
       </c>
     </row>
@@ -14516,7 +14516,7 @@
       </c>
       <c r="C397" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -14535,7 +14535,7 @@
       </c>
       <c r="C398" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -14554,7 +14554,7 @@
       </c>
       <c r="C399" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -15590,7 +15590,7 @@
       </c>
       <c r="C411" t="inlineStr">
         <is>
-          <t>Запрос направлен</t>
+          <t>Взыскание обращено</t>
         </is>
       </c>
     </row>
@@ -15759,7 +15759,7 @@
       </c>
       <c r="C420" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -16090,7 +16090,7 @@
       </c>
       <c r="C438" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Запрос направлен</t>
         </is>
       </c>
     </row>
@@ -16180,7 +16180,7 @@
       </c>
       <c r="C443" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -16233,7 +16233,7 @@
       </c>
       <c r="C446" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Взыскание обращено</t>
         </is>
       </c>
     </row>
@@ -16375,7 +16375,7 @@
       </c>
       <c r="C454" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -16428,7 +16428,7 @@
       </c>
       <c r="C457" t="inlineStr">
         <is>
-          <t>Обращение рассмотрено</t>
+          <t>Запрос направлен</t>
         </is>
       </c>
     </row>
@@ -16445,7 +16445,7 @@
       </c>
       <c r="C458" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Взыскание обращено</t>
         </is>
       </c>
     </row>
@@ -16514,7 +16514,7 @@
       </c>
       <c r="C462" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Взыскание обращено</t>
         </is>
       </c>
     </row>
@@ -16531,7 +16531,7 @@
       </c>
       <c r="C463" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Взыскание обращено</t>
         </is>
       </c>
     </row>
@@ -16717,7 +16717,7 @@
       </c>
       <c r="C473" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Взыскание обращено</t>
         </is>
       </c>
     </row>
@@ -17340,7 +17340,7 @@
       </c>
       <c r="C507" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -17357,7 +17357,7 @@
       </c>
       <c r="C508" t="inlineStr">
         <is>
-          <t>Запрос направлен</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -17429,7 +17429,7 @@
       </c>
       <c r="C512" t="inlineStr">
         <is>
-          <t>Запрос направлен</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -17709,7 +17709,7 @@
       </c>
       <c r="C528" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -17726,7 +17726,7 @@
       </c>
       <c r="C529" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Взыскание обращено</t>
         </is>
       </c>
     </row>
@@ -17743,7 +17743,7 @@
       </c>
       <c r="C530" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -17895,7 +17895,7 @@
       </c>
       <c r="C538" t="inlineStr">
         <is>
-          <t>Взыскание обращено</t>
+          <t>Запрос направлен</t>
         </is>
       </c>
     </row>
@@ -17931,7 +17931,7 @@
       </c>
       <c r="C540" t="inlineStr">
         <is>
-          <t>Запрос направлен</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -17984,7 +17984,7 @@
       </c>
       <c r="C543" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -18071,7 +18071,7 @@
       </c>
       <c r="C548" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Запрос направлен</t>
         </is>
       </c>
     </row>
@@ -18298,7 +18298,7 @@
       </c>
       <c r="C560" t="inlineStr">
         <is>
-          <t>Обращение рассмотрено</t>
+          <t>Запрос направлен</t>
         </is>
       </c>
     </row>
@@ -18427,7 +18427,7 @@
       </c>
       <c r="C567" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Взыскание обращено</t>
         </is>
       </c>
     </row>
@@ -18734,7 +18734,7 @@
       </c>
       <c r="C584" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Запрос направлен</t>
         </is>
       </c>
     </row>
@@ -18751,7 +18751,7 @@
       </c>
       <c r="C585" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -18945,7 +18945,7 @@
       </c>
       <c r="C596" t="inlineStr">
         <is>
-          <t>Взыскание обращено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -19167,7 +19167,7 @@
       </c>
       <c r="C607" t="inlineStr">
         <is>
-          <t>Запрос направлен</t>
+          <t>Постановление вынесено</t>
         </is>
       </c>
     </row>
@@ -19410,7 +19410,7 @@
       </c>
       <c r="C620" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -19914,7 +19914,7 @@
       </c>
       <c r="C647" t="inlineStr">
         <is>
-          <t>Запрос направлен</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -19949,7 +19949,7 @@
       </c>
       <c r="C649" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Запрос направлен</t>
         </is>
       </c>
     </row>
@@ -20719,7 +20719,7 @@
       </c>
       <c r="C691" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -20736,7 +20736,7 @@
       </c>
       <c r="C692" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -20850,7 +20850,7 @@
       </c>
       <c r="C698" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Запрос направлен</t>
         </is>
       </c>
     </row>
@@ -20868,7 +20868,7 @@
       </c>
       <c r="C699" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -21062,7 +21062,7 @@
       </c>
       <c r="C710" t="inlineStr">
         <is>
-          <t>Запрос направлен</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -21243,7 +21243,7 @@
       </c>
       <c r="C719" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -21512,7 +21512,7 @@
       </c>
       <c r="C733" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -22048,7 +22048,7 @@
       </c>
       <c r="C748" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Запрос направлен</t>
         </is>
       </c>
     </row>
@@ -22211,7 +22211,7 @@
       </c>
       <c r="C757" t="inlineStr">
         <is>
-          <t>Обращение рассмотрено</t>
+          <t>Взыскание обращено</t>
         </is>
       </c>
     </row>
@@ -22269,7 +22269,7 @@
       </c>
       <c r="C760" t="inlineStr">
         <is>
-          <t>Запрос направлен</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -22562,7 +22562,7 @@
       </c>
       <c r="C773" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -22580,7 +22580,7 @@
       </c>
       <c r="C774" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -22597,7 +22597,7 @@
       </c>
       <c r="C775" t="inlineStr">
         <is>
-          <t>Запрос направлен</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -22848,7 +22848,7 @@
       </c>
       <c r="C789" t="inlineStr">
         <is>
-          <t>Запрет действий</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -22958,7 +22958,7 @@
       </c>
       <c r="C795" t="inlineStr">
         <is>
-          <t>Обращение рассмотрено</t>
+          <t>Взыскание обращено</t>
         </is>
       </c>
     </row>
@@ -23012,7 +23012,7 @@
       </c>
       <c r="C798" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Взыскание обращено</t>
         </is>
       </c>
     </row>
@@ -23030,7 +23030,7 @@
       </c>
       <c r="C799" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Взыскание обращено</t>
         </is>
       </c>
     </row>
@@ -23084,7 +23084,7 @@
       </c>
       <c r="C802" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -23239,7 +23239,7 @@
       </c>
       <c r="C811" t="inlineStr">
         <is>
-          <t>Запрос направлен</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -23386,7 +23386,7 @@
       </c>
       <c r="C819" t="inlineStr">
         <is>
-          <t>Взыскание обращено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -23422,7 +23422,7 @@
       </c>
       <c r="C821" t="inlineStr">
         <is>
-          <t>Обращение рассмотрено</t>
+          <t>Запрос направлен</t>
         </is>
       </c>
     </row>
@@ -23576,7 +23576,7 @@
       </c>
       <c r="C828" t="inlineStr">
         <is>
-          <t>Запрос направлен</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -23886,7 +23886,7 @@
       </c>
       <c r="C844" t="inlineStr">
         <is>
-          <t>Запрет действий</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -23921,7 +23921,7 @@
       </c>
       <c r="C846" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -23956,7 +23956,7 @@
       </c>
       <c r="C848" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Запрос направлен</t>
         </is>
       </c>
     </row>
@@ -24362,7 +24362,7 @@
       </c>
       <c r="C870" t="inlineStr">
         <is>
-          <t>Запрет действий</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -24379,7 +24379,7 @@
       </c>
       <c r="C871" t="inlineStr">
         <is>
-          <t>Запрет действий</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -24496,7 +24496,7 @@
       </c>
       <c r="C877" t="inlineStr">
         <is>
-          <t>Запрос направлен</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -24843,7 +24843,7 @@
       </c>
       <c r="C891" t="inlineStr">
         <is>
-          <t>Запрос направлен</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -25435,7 +25435,7 @@
       </c>
       <c r="C922" t="inlineStr">
         <is>
-          <t>Запрет действий</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -25950,7 +25950,7 @@
       </c>
       <c r="C951" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Запрос направлен</t>
         </is>
       </c>
     </row>
@@ -26418,7 +26418,7 @@
       </c>
       <c r="C975" t="inlineStr">
         <is>
-          <t>Обращение рассмотрено</t>
+          <t>Запрос направлен</t>
         </is>
       </c>
     </row>
@@ -26469,7 +26469,7 @@
       </c>
       <c r="C978" t="inlineStr">
         <is>
-          <t>Постановление вынесено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -26637,7 +26637,7 @@
       </c>
       <c r="C987" t="inlineStr">
         <is>
-          <t>Запрос направлен</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -26734,7 +26734,7 @@
       </c>
       <c r="C992" t="inlineStr">
         <is>
-          <t>Взыскание обращено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>
@@ -26823,7 +26823,7 @@
       </c>
       <c r="C997" t="inlineStr">
         <is>
-          <t>Взыскание обращено</t>
+          <t>Обращение рассмотрено</t>
         </is>
       </c>
     </row>

</xml_diff>